<commit_message>
before we go mymenshingh
</commit_message>
<xml_diff>
--- a/Milk account.xlsx
+++ b/Milk account.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                   Due=50</t>
+  </si>
+  <si>
+    <t>0gm</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +422,7 @@
       </c>
       <c r="D2">
         <f>SUM(C2:C93)</f>
-        <v>270</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,6 +563,54 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f>DATE(2021,5,7)</f>
+        <v>44323</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f>DATE(2021,5,8)</f>
+        <v>44324</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f>DATE(2021,5,9)</f>
+        <v>44325</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f>DATE(2021,5,10)</f>
+        <v>44326</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>